<commit_message>
Add data from Friday lab section
</commit_message>
<xml_diff>
--- a/bmes301/lab2/data/lab2_specimen_dimensions.xlsx
+++ b/bmes301/lab2/data/lab2_specimen_dimensions.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/178c4c426960fab1/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-22.04\home\kabil\sietch\courses\bmes301\lab2\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{54557BAD-A1F6-42F4-8A5A-AEE329A274C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D70A662D-985E-45BF-B74B-B2FCDA203B07}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{DFB77BC6-F6E8-445C-A178-3DB32BAD6500}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31695" yWindow="1950" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -60,7 +60,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -83,6 +83,12 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -104,7 +110,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -136,11 +142,50 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -164,6 +209,17 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -472,7 +528,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E17" sqref="E17"/>
+      <selection pane="bottomLeft" activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -485,7 +541,7 @@
     <col min="6" max="6" width="9.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -502,7 +558,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -585,46 +641,76 @@
       <c r="A7" s="6">
         <v>6</v>
       </c>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
+      <c r="B7" s="7">
+        <v>24.1</v>
+      </c>
+      <c r="C7" s="7">
+        <v>7.1</v>
+      </c>
+      <c r="D7" s="7">
+        <v>0.5</v>
+      </c>
       <c r="E7" s="7"/>
     </row>
     <row r="8" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>7</v>
       </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
+      <c r="B8" s="2">
+        <v>14.8</v>
+      </c>
+      <c r="C8" s="2">
+        <v>6.2</v>
+      </c>
+      <c r="D8" s="2">
+        <v>0.5</v>
+      </c>
       <c r="E8" s="4"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="6">
         <v>8</v>
       </c>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
+      <c r="B9" s="7">
+        <v>14.7</v>
+      </c>
+      <c r="C9" s="7">
+        <v>7.6</v>
+      </c>
+      <c r="D9" s="7">
+        <v>0.8</v>
+      </c>
       <c r="E9" s="7"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>9</v>
       </c>
-      <c r="B10" s="4"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
+      <c r="B10" s="14">
+        <v>13.6</v>
+      </c>
+      <c r="C10" s="15">
+        <v>5.7</v>
+      </c>
+      <c r="D10" s="15">
+        <v>1.1000000000000001</v>
+      </c>
       <c r="E10" s="4"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="6">
+      <c r="A11" s="12">
         <v>10</v>
       </c>
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
+      <c r="B11" s="11">
+        <v>21.5</v>
+      </c>
+      <c r="C11" s="11">
+        <v>6</v>
+      </c>
+      <c r="D11" s="11">
+        <v>0.5</v>
+      </c>
+      <c r="E11" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>